<commit_message>
update behavioral data to participant 312
</commit_message>
<xml_diff>
--- a/data/subjects.xlsx
+++ b/data/subjects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpotier/BienJoue/BJAnal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FF1CEE-6C32-6642-8666-2A10175EA15F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B9336C-6C42-CE45-B623-6215683D874C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4CA2F768-A5D5-E44D-8C86-B547C0D367B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{4CA2F768-A5D5-E44D-8C86-B547C0D367B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$137</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A4BB99-83C1-A547-81AF-617F12988F8C}">
   <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I137"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
clean data to 321
</commit_message>
<xml_diff>
--- a/data/subjects.xlsx
+++ b/data/subjects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpotier/BienJoue/BJAnal/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B9336C-6C42-CE45-B623-6215683D874C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E600185D-4DE1-CD49-BDC6-2E40E070A6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{4CA2F768-A5D5-E44D-8C86-B547C0D367B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4CA2F768-A5D5-E44D-8C86-B547C0D367B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="177">
   <si>
     <t>subj_num</t>
   </si>
@@ -475,6 +475,90 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>mbse2ual93</t>
+  </si>
+  <si>
+    <t>zvtxod636o</t>
+  </si>
+  <si>
+    <t>v7hpnfwykc</t>
+  </si>
+  <si>
+    <t>ekge7117c0</t>
+  </si>
+  <si>
+    <t>vfdk659lm2</t>
+  </si>
+  <si>
+    <t>dyhqkv4y90</t>
+  </si>
+  <si>
+    <t>ellh3f7r6f</t>
+  </si>
+  <si>
+    <t>b0n958l42w</t>
+  </si>
+  <si>
+    <t>dmcfba923s</t>
+  </si>
+  <si>
+    <t>8jm4ktdp2v</t>
+  </si>
+  <si>
+    <t>g3h6mfmlh9</t>
+  </si>
+  <si>
+    <t>bvzbcex95y</t>
+  </si>
+  <si>
+    <t>sedpugnmk5</t>
+  </si>
+  <si>
+    <t>6ee8c6wkk7</t>
+  </si>
+  <si>
+    <t>a8fzyae532</t>
+  </si>
+  <si>
+    <t>7xjxwvk39u</t>
+  </si>
+  <si>
+    <t>37uuqlft2a</t>
+  </si>
+  <si>
+    <t>qgecou8jlo</t>
+  </si>
+  <si>
+    <t>z4rx8bqocr</t>
+  </si>
+  <si>
+    <t>ma2hmr7lqa</t>
+  </si>
+  <si>
+    <t>6tavb9lkp3</t>
+  </si>
+  <si>
+    <t>b2jojnaqxl</t>
+  </si>
+  <si>
+    <t>50ppjg6by9</t>
+  </si>
+  <si>
+    <t>o8rq1gza2t</t>
+  </si>
+  <si>
+    <t>wtc1en8xqx</t>
+  </si>
+  <si>
+    <t>24mprbt056</t>
+  </si>
+  <si>
+    <t>s5qctl4onx</t>
+  </si>
+  <si>
+    <t>fzegt6t3y1</t>
   </si>
 </sst>
 </file>
@@ -517,12 +601,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -543,7 +630,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -839,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A4BB99-83C1-A547-81AF-617F12988F8C}">
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="H164" sqref="H164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2384,6 +2471,314 @@
         <v>99</v>
       </c>
     </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>315</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>315</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>315</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>315</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>316</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>316</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>316</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>316</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>317</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>317</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>317</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>317</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>318</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>318</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>318</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>318</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>319</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>319</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>319</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>319</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>320</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>320</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>320</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>320</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>321</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>321</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>321</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>321</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I137" xr:uid="{CB0864BB-5719-934E-B410-69FC3123B5E8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>